<commit_message>
add control map and player prefab
</commit_message>
<xml_diff>
--- a/planning prévisionnel.xlsx
+++ b/planning prévisionnel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vehel\Documents\projet_unity\porte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF81B975-2FB1-4138-B3DD-D49A9A76D068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC53B69-41AA-4874-B261-4D51EBE7579F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3648" yWindow="720" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1776" yWindow="720" windowWidth="19152" windowHeight="9348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -293,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -301,10 +301,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -324,10 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -615,16 +612,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="32.44140625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="3" max="4" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="12.21875" customWidth="1"/>
     <col min="10" max="10" width="18.21875" customWidth="1"/>
@@ -671,141 +667,141 @@
       <c r="D4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="16"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="15"/>
     </row>
     <row r="5" spans="2:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="13"/>
-      <c r="D5" s="15"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="16"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="15"/>
     </row>
     <row r="6" spans="2:12" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="13"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="16"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="15"/>
     </row>
     <row r="7" spans="2:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="13"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="16"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="15"/>
     </row>
     <row r="8" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="13"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="H8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="15"/>
     </row>
     <row r="9" spans="2:12" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="13"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="16"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="15"/>
     </row>
     <row r="10" spans="2:12" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
       <c r="J10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="16"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="15"/>
     </row>
     <row r="11" spans="2:12" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="13"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
       <c r="K11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="16"/>
+      <c r="L11" s="15"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -814,7 +810,7 @@
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
-      <c r="L12" s="18" t="s">
+      <c r="L12" s="17" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>